<commit_message>
Updated for TC003(new Scenario)
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/MastekBlanketPOM/data/AssignLeave.xlsx
+++ b/src/main/java/com/test/automation/MastekBlanketPOM/data/AssignLeave.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
   <si>
     <t>TestCase</t>
   </si>
@@ -45,48 +45,18 @@
     <t>Y</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>IsMultipleEmployee</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>subUnit</t>
-  </si>
-  <si>
     <t>EmployeeName</t>
   </si>
   <si>
     <t>LeaveType</t>
   </si>
   <si>
-    <t>LeavePeriod</t>
-  </si>
-  <si>
-    <t>Entitlement</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
     <t>Maternity US</t>
   </si>
   <si>
-    <t>2017-01-01 - 2017-12-31</t>
-  </si>
-  <si>
     <t>Vacation US</t>
   </si>
   <si>
-    <t>2018-01-01 - 2018-12-31</t>
-  </si>
-  <si>
     <t>TC004</t>
   </si>
   <si>
@@ -193,9 +163,6 @@
   </si>
   <si>
     <t>-20</t>
-  </si>
-  <si>
-    <t>Linda</t>
   </si>
   <si>
     <t>John</t>
@@ -518,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,52 +520,52 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="P1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" t="s">
         <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -609,25 +576,25 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="P2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -638,99 +605,22 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="R3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" t="s">
-        <v>45</v>
-      </c>
-      <c r="P4" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q5" s="1"/>
-      <c r="R5" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -740,10 +630,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="A1:XFD1048576"/>
+      <selection sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +649,7 @@
     <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -767,28 +657,55 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -796,22 +713,28 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -819,22 +742,25 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
+        <v>27</v>
+      </c>
+      <c r="R3" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -842,45 +768,73 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" s="1"/>
+      <c r="R5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>